<commit_message>
Converted data to csv files
</commit_message>
<xml_diff>
--- a/All Thr.xlsx
+++ b/All Thr.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/luigi_guiducci3_unibo_it/Documents/LabNSN2_2022-23/Groups/3R/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Lab2_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="237" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96B72358-6AA8-48D8-922D-BAE94DBD15C2}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2775" windowWidth="20085" windowHeight="10980" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2592" yWindow="2772" windowWidth="20088" windowHeight="10980" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PMTs_1-2" sheetId="6" r:id="rId1"/>
@@ -152,7 +151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -190,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -202,6 +201,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -234,6 +234,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -259,7 +260,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -309,10 +310,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'PMTs_7-8'!$B$9:$B$29</c:f>
+              <c:f>'PMTs_7-8'!$B$9:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -353,27 +354,12 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -381,10 +367,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PMTs_7-8'!$C$9:$C$29</c:f>
+              <c:f>'PMTs_7-8'!$C$9:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>83657</c:v>
                 </c:pt>
@@ -424,13 +410,13 @@
                 <c:pt idx="12">
                   <c:v>3011</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>2263</c:v>
+                </c:pt>
                 <c:pt idx="14">
-                  <c:v>2263</c:v>
-                </c:pt>
-                <c:pt idx="16">
                   <c:v>1681</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="15">
                   <c:v>789</c:v>
                 </c:pt>
               </c:numCache>
@@ -509,7 +495,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2010883856"/>
@@ -571,7 +557,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2010882608"/>
@@ -612,7 +598,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -638,6 +624,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -663,7 +650,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -713,10 +700,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'PMTs_7-8'!$B$9:$B$29</c:f>
+              <c:f>'PMTs_7-8'!$B$9:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -757,27 +744,12 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -785,10 +757,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PMTs_7-8'!$D$9:$D$29</c:f>
+              <c:f>'PMTs_7-8'!$D$9:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>34370</c:v>
                 </c:pt>
@@ -828,13 +800,13 @@
                 <c:pt idx="12">
                   <c:v>1031</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>656</c:v>
+                </c:pt>
                 <c:pt idx="14">
-                  <c:v>656</c:v>
-                </c:pt>
-                <c:pt idx="16">
                   <c:v>407</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="15">
                   <c:v>146</c:v>
                 </c:pt>
               </c:numCache>
@@ -913,7 +885,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2012174000"/>
@@ -975,7 +947,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2012170256"/>
@@ -1016,7 +988,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1042,6 +1014,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1067,7 +1040,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1117,10 +1090,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'PMTs_7-8'!$B$9:$B$29</c:f>
+              <c:f>'PMTs_7-8'!$B$9:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1161,27 +1134,12 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1189,10 +1147,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PMTs_7-8'!$E$9:$E$29</c:f>
+              <c:f>'PMTs_7-8'!$E$9:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>5867</c:v>
                 </c:pt>
@@ -1232,13 +1190,13 @@
                 <c:pt idx="12">
                   <c:v>1495</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>1326</c:v>
+                </c:pt>
                 <c:pt idx="14">
-                  <c:v>1326</c:v>
-                </c:pt>
-                <c:pt idx="16">
                   <c:v>1128</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="15">
                   <c:v>628</c:v>
                 </c:pt>
               </c:numCache>
@@ -1317,7 +1275,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2012174416"/>
@@ -1379,7 +1337,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2012175248"/>
@@ -1420,7 +1378,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1446,6 +1404,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1471,7 +1430,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1521,10 +1480,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'PMTs_7-8'!$B$9:$B$29</c:f>
+              <c:f>'PMTs_7-8'!$B$9:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1565,27 +1524,12 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1593,10 +1537,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PMTs_7-8'!$F$9:$F$29</c:f>
+              <c:f>'PMTs_7-8'!$F$9:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>3692</c:v>
                 </c:pt>
@@ -1636,13 +1580,13 @@
                 <c:pt idx="12">
                   <c:v>756</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>497</c:v>
+                </c:pt>
                 <c:pt idx="14">
-                  <c:v>497</c:v>
-                </c:pt>
-                <c:pt idx="16">
                   <c:v>313</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="15">
                   <c:v>106</c:v>
                 </c:pt>
               </c:numCache>
@@ -1721,7 +1665,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2006122608"/>
@@ -1783,7 +1727,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2006123440"/>
@@ -1824,7 +1768,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1875,7 +1819,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2093,7 +2037,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1776603744"/>
@@ -2155,7 +2099,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1776602912"/>
@@ -2172,6 +2116,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2179,7 +2124,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2203,7 +2147,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5480,39 +5424,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6214D89-4229-471F-B79A-D771C07BEDED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5520,7 +5464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -5528,7 +5472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -5536,10 +5480,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5562,39 +5506,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F074A2D-B561-451B-BE25-AC6C83664406}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5602,7 +5546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -5610,7 +5554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -5618,10 +5562,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5644,39 +5588,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BCE458E-2008-42C4-A466-4BB7C2F8C884}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5684,7 +5628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -5692,7 +5636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -5700,10 +5644,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5726,21 +5670,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F46802-D4CB-4090-952D-90A1E5EFEBF9}">
-  <dimension ref="A1:F29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5748,7 +5692,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -5756,7 +5700,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -5764,7 +5708,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5775,7 +5719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -5786,7 +5730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -5797,10 +5741,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5817,7 +5761,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>3</v>
       </c>
@@ -5834,7 +5778,7 @@
         <v>3692</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>5</v>
       </c>
@@ -5851,7 +5795,7 @@
         <v>2964</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>10</v>
       </c>
@@ -5868,7 +5812,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>15</v>
       </c>
@@ -5885,7 +5829,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>20</v>
       </c>
@@ -5902,7 +5846,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>25</v>
       </c>
@@ -5919,7 +5863,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>30</v>
       </c>
@@ -5936,7 +5880,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>35</v>
       </c>
@@ -5953,7 +5897,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>40</v>
       </c>
@@ -5970,7 +5914,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>45</v>
       </c>
@@ -5987,7 +5931,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>50</v>
       </c>
@@ -6004,7 +5948,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>55</v>
       </c>
@@ -6021,7 +5965,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>60</v>
       </c>
@@ -6038,79 +5982,54 @@
         <v>756</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="C22">
+        <v>2263</v>
+      </c>
+      <c r="D22">
+        <v>656</v>
+      </c>
+      <c r="E22">
+        <v>1326</v>
+      </c>
+      <c r="F22">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C23">
-        <v>2263</v>
+        <v>1681</v>
       </c>
       <c r="D23">
-        <v>656</v>
+        <v>407</v>
       </c>
       <c r="E23">
-        <v>1326</v>
+        <v>1128</v>
       </c>
       <c r="F23">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>80</v>
-      </c>
-      <c r="C25">
-        <v>1681</v>
-      </c>
-      <c r="D25">
-        <v>407</v>
-      </c>
-      <c r="E25">
-        <v>1128</v>
-      </c>
-      <c r="F25">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29">
         <v>100</v>
       </c>
-      <c r="C29">
+      <c r="C24">
         <v>789</v>
       </c>
-      <c r="D29">
+      <c r="D24">
         <v>146</v>
       </c>
-      <c r="E29">
+      <c r="E24">
         <v>628</v>
       </c>
-      <c r="F29">
+      <c r="F24">
         <v>106</v>
       </c>
     </row>
@@ -6121,41 +6040,41 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50332F3-F886-4B18-9B6E-359E86759B4E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -6163,7 +6082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -6171,7 +6090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -6179,10 +6098,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -6205,21 +6124,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6227,7 +6146,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -6235,7 +6154,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -6243,7 +6162,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -6254,7 +6173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -6265,7 +6184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -6276,10 +6195,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -6296,7 +6215,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>5</v>
       </c>
@@ -6313,7 +6232,7 @@
         <v>3075</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -6330,7 +6249,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>10</v>
       </c>
@@ -6347,7 +6266,7 @@
         <v>2341</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>15</v>
       </c>
@@ -6364,7 +6283,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>20</v>
       </c>
@@ -6381,7 +6300,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>25</v>
       </c>
@@ -6398,7 +6317,7 @@
         <v>1712</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>30</v>
       </c>
@@ -6415,7 +6334,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>32</v>
       </c>
@@ -6432,7 +6351,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>35</v>
       </c>
@@ -6449,7 +6368,7 @@
         <v>1563</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>40</v>
       </c>
@@ -6466,7 +6385,7 @@
         <v>1623</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>41</v>
       </c>
@@ -6483,7 +6402,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>45</v>
       </c>
@@ -6500,7 +6419,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>50</v>
       </c>
@@ -6517,7 +6436,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>60</v>
       </c>
@@ -6534,7 +6453,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>70</v>
       </c>

</xml_diff>